<commit_message>
Creates only first child dimension. Still working on role playing.
</commit_message>
<xml_diff>
--- a/Documentation/ExtendedPropertiesList.xlsx
+++ b/Documentation/ExtendedPropertiesList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="96">
   <si>
     <t>AdditionalColumnDefinitionStaging1</t>
   </si>
@@ -306,6 +306,12 @@
   </si>
   <si>
     <t>Exclude from traversing the related tables via this column for flattening</t>
+  </si>
+  <si>
+    <t>PrimaryRelationship</t>
+  </si>
+  <si>
+    <t>Ordering of columns where multiple rol playing dimensions exist. E.g. Which table will also be used for DimUser as well as DimApprovingUser</t>
   </si>
 </sst>
 </file>
@@ -626,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,55 +955,55 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>48</v>
+      <c r="C23" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="1" t="b">
-        <v>1</v>
+      <c r="C24" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>49</v>
+      <c r="C25" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D26" t="s">
         <v>77</v>
@@ -1005,13 +1011,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D27" t="s">
         <v>77</v>
@@ -1019,105 +1025,105 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B29" t="s">
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
         <v>1</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="D30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B31" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="1" t="b">
-        <v>1</v>
+      <c r="C31" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="D31" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B32" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>54</v>
+      <c r="C32" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B33" t="s">
         <v>1</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="1" t="b">
-        <v>1</v>
+      <c r="C34" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="D34" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B35" t="s">
         <v>1</v>
@@ -1126,12 +1132,12 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B36" t="s">
         <v>1</v>
@@ -1140,12 +1146,12 @@
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B37" t="s">
         <v>1</v>
@@ -1154,76 +1160,90 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B38" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>56</v>
+      <c r="C38" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B39" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="1">
-        <v>1</v>
+      <c r="C39" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="D39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B40" t="s">
         <v>1</v>
       </c>
       <c r="C40" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B41" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>57</v>
+      <c r="C41" s="1">
+        <v>9</v>
       </c>
       <c r="D41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>38</v>
       </c>
-      <c r="B42" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>